<commit_message>
added PhPrice for every client
</commit_message>
<xml_diff>
--- a/Database/Phar.xlsx
+++ b/Database/Phar.xlsx
@@ -14,14 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>صيدلية العقباوى</t>
-  </si>
-  <si>
     <t>صيدلية النورس</t>
   </si>
   <si>
@@ -34,10 +31,7 @@
     <t>صيدلية د.سامي سمير</t>
   </si>
   <si>
-    <t>صيدلية د.شريف</t>
-  </si>
-  <si>
-    <t>صيدلية د.عبد الله كامل</t>
+    <t>صيدلية د.شريف نوح</t>
   </si>
   <si>
     <t>صيدلية د.كامل مرعي</t>
@@ -56,6 +50,57 @@
   </si>
   <si>
     <t>صيدلية د.وفاء عبده</t>
+  </si>
+  <si>
+    <t>صيدلية العقباوى القاهرة</t>
+  </si>
+  <si>
+    <t>صيدلية د.وليد</t>
+  </si>
+  <si>
+    <t>صيدلية د. عبد الله كامل - القاهرة</t>
+  </si>
+  <si>
+    <t>صيدلية د.هبة - القاهرة</t>
+  </si>
+  <si>
+    <t>صيدلية د.أسماء - القاهرة</t>
+  </si>
+  <si>
+    <t>صيدلية 70 فدان</t>
+  </si>
+  <si>
+    <t>صيدلية العبور</t>
+  </si>
+  <si>
+    <t>صيدلية د.احمد احمد</t>
+  </si>
+  <si>
+    <t>صيدلية العبور - القاهرة</t>
+  </si>
+  <si>
+    <t>صيدلية د.ابراهيم</t>
+  </si>
+  <si>
+    <t>صيدلية الصفا والمروة</t>
+  </si>
+  <si>
+    <t>صيدلية د. نعيم</t>
+  </si>
+  <si>
+    <t>صيدلية د.اسماء - القاهرة</t>
+  </si>
+  <si>
+    <t>صيدلية د.شيماء</t>
+  </si>
+  <si>
+    <t>صيدلية /د.عادل سعيد</t>
+  </si>
+  <si>
+    <t>كوزى كورنر</t>
+  </si>
+  <si>
+    <t>صيدلية الحرية - القاهرة</t>
   </si>
 </sst>
 </file>
@@ -413,7 +458,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -528,6 +573,126 @@
         <v>13</v>
       </c>
     </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>